<commit_message>
change files of academic advising
</commit_message>
<xml_diff>
--- a/Studetn_inst_AcademicAdvisor.xlsx
+++ b/Studetn_inst_AcademicAdvisor.xlsx
@@ -26,18 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>mail</t>
-  </si>
-  <si>
-    <t>Name Instructor</t>
-  </si>
-  <si>
-    <t>mail Instructor</t>
-  </si>
-  <si>
     <t>Osama Mohamed Youssef Selim Ibrahim</t>
   </si>
   <si>
@@ -81,6 +69,18 @@
   </si>
   <si>
     <t>dshawky@zewailcity.edu.eg</t>
+  </si>
+  <si>
+    <t>Student Name</t>
+  </si>
+  <si>
+    <t>Student Mail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructor Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instructor Mail </t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,86 +449,86 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>